<commit_message>
Updated with some graphs.
</commit_message>
<xml_diff>
--- a/scaling.xlsx
+++ b/scaling.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Scaling</t>
   </si>
@@ -82,13 +82,25 @@
   </si>
   <si>
     <t>read GCC 4.8 x64 4 core 2 thread Intel i7-3770K @ 3.50Ghz</t>
+  </si>
+  <si>
+    <t>write VS2013 x64 4 core 8 thread Intel i7-3770K @ 3.50Ghz</t>
+  </si>
+  <si>
+    <t>read VS2013 x64 4 core 8 thread Intel i7-3770K @ 3.50Ghz</t>
+  </si>
+  <si>
+    <t>GCC 4.8 write over VS2013 write</t>
+  </si>
+  <si>
+    <t>GCC 4.8 write over VS2013 read</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +110,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,9 +145,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,7 +160,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:lang val="en-IE"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -212,7 +233,7 @@
                   <c:v>2.0299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2324573678660347</c:v>
+                  <c:v>4.108015668156451</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -264,7 +285,7 @@
                   <c:v>2.2799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7171385875945036</c:v>
+                  <c:v>4.0641002807025517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -375,11 +396,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="216567808"/>
-        <c:axId val="216570112"/>
+        <c:axId val="155215744"/>
+        <c:axId val="155246976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="216567808"/>
+        <c:axId val="155215744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8"/>
@@ -406,12 +427,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216570112"/>
+        <c:crossAx val="155246976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="216570112"/>
+        <c:axId val="155246976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,7 +458,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216567808"/>
+        <c:crossAx val="155215744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -450,7 +471,242 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-IE"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>By</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> h</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>ow</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IE" baseline="0"/>
+              <a:t> many times GCC 4.8 is faster than VS2013 for proposed boost::concurrent_unordered_map</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-IE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GCC 4.8 write over VS2013 write</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$46:$D$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$47:$D$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.6355409885859462</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8277398489160299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4627182188102421</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GCC 4.8 write over VS2013 read</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$46:$D$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$48:$D$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.0162929712865756</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.145046759330449</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7616136846524511</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="61684736"/>
+        <c:axId val="61683200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="61684736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>CPU</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IE" baseline="0"/>
+                  <a:t> cores</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61683200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="61683200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>How</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IE" baseline="0"/>
+                  <a:t> many times faster</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61684736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -460,16 +716,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -483,6 +739,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -776,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1051,6 +1337,50 @@
         <v>44057236</v>
       </c>
     </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:B15" si="5">C14/D14</f>
+        <v>0.22979036330042299</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:C15" si="6">H14/E14</f>
+        <v>0.91916145320169196</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>19897995</v>
+      </c>
+      <c r="H14">
+        <v>18289470</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="5"/>
+        <v>0.25193952196510783</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="6"/>
+        <v>1.0077580878604313</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>42025175</v>
+      </c>
+      <c r="H15">
+        <v>42351210</v>
+      </c>
+    </row>
     <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>7</v>
@@ -1116,7 +1446,7 @@
         <v>3</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:B25" si="5">C22/D22</f>
+        <f t="shared" ref="B22:B25" si="7">C22/D22</f>
         <v>0.66724769650476523</v>
       </c>
       <c r="C22">
@@ -1138,7 +1468,7 @@
         <v>8</v>
       </c>
       <c r="B23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0581143419665087</v>
       </c>
       <c r="C23">
@@ -1160,7 +1490,7 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.67928464689862589</v>
       </c>
       <c r="C24">
@@ -1182,7 +1512,7 @@
         <v>11</v>
       </c>
       <c r="B25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1.0135408146164182</v>
       </c>
       <c r="C25">
@@ -1204,7 +1534,7 @@
         <v>12</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26" si="6">C26/D26</f>
+        <f t="shared" ref="B26" si="8">C26/D26</f>
         <v>1.1386400727311314</v>
       </c>
       <c r="C26">
@@ -1226,7 +1556,7 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27:B28" si="7">C27/D27</f>
+        <f t="shared" ref="B27:B28" si="9">C27/D27</f>
         <v>0.82649261739877888</v>
       </c>
       <c r="C27">
@@ -1248,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="B28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.78270001784300591</v>
       </c>
       <c r="C28">
@@ -1270,11 +1600,11 @@
         <v>18</v>
       </c>
       <c r="B29">
-        <f t="shared" ref="B29:B32" si="8">C29/D29</f>
+        <f t="shared" ref="B29:B32" si="10">C29/D29</f>
         <v>0.89066037786421004</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:C30" si="9">H29/E29</f>
+        <f t="shared" ref="C29:C30" si="11">H29/E29</f>
         <v>3.5626415114568402</v>
       </c>
       <c r="D29">
@@ -1292,11 +1622,11 @@
         <v>19</v>
       </c>
       <c r="B30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.88769027768285569</v>
       </c>
       <c r="C30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>3.5507611107314228</v>
       </c>
       <c r="D30">
@@ -1310,51 +1640,95 @@
       </c>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B31">
-        <f t="shared" si="8"/>
+      <c r="B31" s="2">
+        <f t="shared" si="10"/>
         <v>0.89254140130050619</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <f>F31/E31</f>
         <v>1.7850828026010124</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>2</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>22012352</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>39293871</v>
       </c>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B32">
-        <f t="shared" si="8"/>
+      <c r="B32" s="2">
+        <f t="shared" si="10"/>
         <v>0.88769027768285569</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <f>C30/2</f>
         <v>1.7753805553657114</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>2</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>48826601</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <f>H30/2</f>
         <v>86685798</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:B34" si="12">C33/D33</f>
+        <v>0.99589349211171696</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:C34" si="13">H33/E33</f>
+        <v>3.9835739684468678</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>13458759</v>
+      </c>
+      <c r="H33">
+        <v>53613962</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="12"/>
+        <v>1.0160250701756379</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="13"/>
+        <v>4.0641002807025517</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>24216025</v>
+      </c>
+      <c r="H34">
+        <v>98416354</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="B40">
         <v>1</v>
       </c>
@@ -1368,7 +1742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1379,11 +1753,11 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="D41">
-        <f>C23</f>
-        <v>4.2324573678660347</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <f>(C23+C33)/2</f>
+        <v>4.108015668156451</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -1394,11 +1768,11 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="D42">
-        <f>C24</f>
-        <v>2.7171385875945036</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <f>C34</f>
+        <v>4.0641002807025517</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1414,7 +1788,7 @@
         <v>3.5626415114568402</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -1428,6 +1802,54 @@
       <c r="D44">
         <f>C30</f>
         <v>3.5507611107314228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <f>E29/E33</f>
+        <v>1.6355409885859462</v>
+      </c>
+      <c r="C47" s="2">
+        <f>E31/E25/(3.5/2.53)</f>
+        <v>1.8277398489160299</v>
+      </c>
+      <c r="D47">
+        <f>H29/H33</f>
+        <v>1.4627182188102421</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <f>E30/E34</f>
+        <v>2.0162929712865756</v>
+      </c>
+      <c r="C48" s="2">
+        <f>E32/E26/(3.5/2.53)</f>
+        <v>2.145046759330449</v>
+      </c>
+      <c r="D48">
+        <f>H30/H34</f>
+        <v>1.7616136846524511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>